<commit_message>
Enrea Gestão de Projeto e IA
</commit_message>
<xml_diff>
--- a/documentos/Entrega 1/Gestão de Projetos/ANALISE DE STAKEOLDER.xlsx
+++ b/documentos/Entrega 1/Gestão de Projetos/ANALISE DE STAKEOLDER.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\23025273\Documents\GitHub\Projeto2\documentos\Entrega 1\Gestão de Projetos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A0B95B2-5D76-4813-9769-F6B568DFABC3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0724763-C985-4836-842F-FABDD8C462E5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9405" tabRatio="854" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -647,48 +647,18 @@
     <t>Resolver problemas dos usuários e fornecer suporte.</t>
   </si>
   <si>
-    <t>Resolução rápida de problemas, satisfação do cliente.</t>
-  </si>
-  <si>
-    <t>Satisfação do cliente, melhoria contínua do suporte.</t>
-  </si>
-  <si>
-    <t>Podem influenciar a satisfação do cliente.</t>
-  </si>
-  <si>
-    <t>Mantêm os clientes satisfeitos e engajados.</t>
-  </si>
-  <si>
-    <t>Responder a perguntas, resolver problemas, coletar feedback do cliente.</t>
-  </si>
-  <si>
-    <t>Fornecer suporte eficaz para manter os clientes felizes.</t>
-  </si>
-  <si>
     <t>Gerência Executiva/Alta Administração</t>
   </si>
   <si>
-    <t>Alinhar o aplicativo com a visão da empresa e garantir o sucesso financeiro e da marca no mercado.</t>
-  </si>
-  <si>
-    <t>Crescimento do aplicativo, alinhamento estratégico, retorno sobre o investimento.</t>
-  </si>
-  <si>
     <t>Sucesso da empresa, crescimento financeiro.</t>
   </si>
   <si>
     <t>Definem a estratégia e os recursos disponíveis.</t>
   </si>
   <si>
-    <t>Determinam o curso do aplicativo e seu impacto na empresa.</t>
-  </si>
-  <si>
     <t>Estabelecer metas estratégicas, alocar recursos, tomar decisões de alto nível.</t>
   </si>
   <si>
-    <t>Manter o alinhamento estratégico e garantir que o aplicativo contribua para os objetivos da empresa.</t>
-  </si>
-  <si>
     <t>Objetivos</t>
   </si>
   <si>
@@ -785,9 +755,6 @@
     <t>Sponsor</t>
   </si>
   <si>
-    <t>Atulizado Em</t>
-  </si>
-  <si>
     <t>SAÚDE E BEM-ESTAR</t>
   </si>
   <si>
@@ -801,12 +768,6 @@
   </si>
   <si>
     <t>6.20.23</t>
-  </si>
-  <si>
-    <t>Reuniões trimestrais no teams de revisão executiva, relatórios executivos resumidos com dados do PBI via ppt.</t>
-  </si>
-  <si>
-    <t>Reuniões mensais no teams de revisão de suporte, resumos enviados por e-mail.</t>
   </si>
   <si>
     <t>Reuniões remotas, relatórios enviados por e-mail.</t>
@@ -859,21 +820,12 @@
     <t>Time Comercial (Sales)</t>
   </si>
   <si>
-    <t>Promover o site e a marca  e atrair novos clientes e possiveis investidores</t>
-  </si>
-  <si>
     <t xml:space="preserve">Aumentar a conscientização, gerar feedback, criar campanhas eficazes para atrair novos clientes. </t>
   </si>
   <si>
-    <t>Moldam a percepção da solução web e da marca no mercado, podendo atingir milhares de usuários no Brasil, podendo espandir para o mercado internacional</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Afetam diretamente a aquisição de novos usuários e no resultado da empresa de conquistar um nome forte no mercado.</t>
   </si>
   <si>
-    <t>Comunicar os benefícios do site aos clientes, coletar feedbaks para melhorias continuas</t>
-  </si>
-  <si>
     <t>Análises aprofundadas de desempenho de campanhas focadas nos usuários.</t>
   </si>
   <si>
@@ -881,80 +833,128 @@
   </si>
   <si>
     <t>Criar designs intuitivos e otimizar a navegação.</t>
+  </si>
+  <si>
+    <t>Design de interface, teste de usabilidade e feedback de design.</t>
+  </si>
+  <si>
+    <t>Colaborar com os desenvolvedores para implementar designs eficazes, voltados para o usuário.</t>
+  </si>
+  <si>
+    <t>Alinhamentos semanais de sprint com a equipe de desenvolvimento, UX utilizando metodologias ágeis.</t>
+  </si>
+  <si>
+    <t>Semanais durante a sprint e as demais reuniões do scrum.</t>
+  </si>
+  <si>
+    <t>Reuniões virtuais E relatórios enviados por e-mail</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Melhorar a experiencia do Usuário na busca pelo melhor custo em viagens por aplicativo. </t>
+  </si>
+  <si>
+    <t>Influenciam o sucesso do site por meio do uso e feedback.</t>
+  </si>
+  <si>
+    <t>Cruciais para a aceitação e popularidade do site.</t>
+  </si>
+  <si>
+    <t>Usar o site, fornecer feedback, compartilhar experiências.</t>
+  </si>
+  <si>
+    <t>Manter os usuários satisfeitos, garantir que o site atenda às suas pesquisas.</t>
+  </si>
+  <si>
+    <t>Comunicar via e-mail, qualquer alteração ou novidade do produto e futuras ofertas</t>
+  </si>
+  <si>
+    <t>Fundamental para o sucesso do site.</t>
+  </si>
+  <si>
+    <t>Relatórios detalhados com métricas específicas e análise de tendências e escolhas.</t>
+  </si>
+  <si>
+    <t>Weekly durante a sprint e as demais reuniões do scrum.</t>
+  </si>
+  <si>
+    <t>Desenvolver um site bem-sucedido que atenda às necessidades dos clientes.</t>
+  </si>
+  <si>
+    <t>Lançamento bem-sucedido, aumento de usuários ativos, satisfação dos clientes.</t>
+  </si>
+  <si>
+    <t>Relatórios de desempenho do site, métricas-chave, feedback dos usuários, status do desenvolvimento.</t>
+  </si>
+  <si>
+    <t>Reuniões semanais e mensais de revisão de desempenho.</t>
+  </si>
+  <si>
+    <t>Resolução rápida de problemas, cumprimento do SLA e  satisfação do cliente.</t>
+  </si>
+  <si>
+    <t>Podem influenciar a satisfação do cliente ao utilizar o serviço.</t>
+  </si>
+  <si>
+    <t>Alinhar o site com a visão da empresa e garantir o sucesso financeiro e da marca no mercado.</t>
+  </si>
+  <si>
+    <t>Determinam o curso do site e seu impacto na empresa.</t>
+  </si>
+  <si>
+    <t>Satisfação do cliente, melhoria contínua do suporte com suporte ao cliente 24h.</t>
+  </si>
+  <si>
+    <t>Fornecer suporte eficaz para manter os clientes satisfeitos.</t>
+  </si>
+  <si>
+    <t>Reuniões mensais de revisão de suporte, resumos enviados por e-mail.</t>
+  </si>
+  <si>
+    <t>Crescimento do site, alinhamento estratégico, retorno sobre o investimento.</t>
+  </si>
+  <si>
+    <t>Manter o alinhamento estratégico e garantir que o site contribua para os objetivos da empresa.</t>
+  </si>
+  <si>
+    <t>Reuniões trimestrais de revisão executiva, relatórios executivos resumidos com dados do PBI via Power Point.</t>
+  </si>
+  <si>
+    <t>Atualizado Em</t>
+  </si>
+  <si>
+    <t>O usuário visualizar e escolher o que melhor atende sua necessidade no momento de realizar uma corrida por aplicativo.</t>
+  </si>
+  <si>
+    <t>Ajudar o maior numero de pessoas de modo fácil rápido e eficiente</t>
+  </si>
+  <si>
+    <t>E-mails de ativação, engajamento, recorrência, News e comunicados gerais.</t>
+  </si>
+  <si>
+    <t>Sucesso do produto, inovação no mercado de comparadores de preços.</t>
+  </si>
+  <si>
+    <t>Promover o site e a marca  e atrair novos clientes e possíveis investidores</t>
+  </si>
+  <si>
+    <t>Moldam a percepção da solução web e da marca no mercado, podendo atingir milhares de usuários no Brasil, podendo expandir para o mercado internacional</t>
+  </si>
+  <si>
+    <t>Comunicar os benefícios do site aos clientes, coletar feedbacks para melhorias continuas</t>
   </si>
   <si>
     <t>Melhorar a usabilidade e a experiência do usuário.
 Construção de personas.
-Pototipação de produtos.</t>
-  </si>
-  <si>
-    <t>Design de interface, teste de usabilidade e feedback de design.</t>
-  </si>
-  <si>
-    <t>Colaborar com os desenvolvedores para implementar designs eficazes, voltados para o usuário.</t>
-  </si>
-  <si>
-    <t>Alinhamentos semanais de sprint com a equipe de desenvolvimento, UX utilizando metodologias ágeis.</t>
-  </si>
-  <si>
-    <t>Semanais durante a sprint e as demais reuniões do scrum.</t>
-  </si>
-  <si>
-    <t>Reuniões virtuais E relatórios enviados por e-mail</t>
-  </si>
-  <si>
-    <t>Reuniões virtuais e dados no GitHub e Figma</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Melhorar a experiencia do Usuário na busca pelo melhor custo em viagens por aplicativo. </t>
-  </si>
-  <si>
-    <t>Ajudar o maior numero de pessoas de modo facil rapido e eficiente</t>
-  </si>
-  <si>
-    <t>Influenciam o sucesso do site por meio do uso e feedback.</t>
-  </si>
-  <si>
-    <t>Cruciais para a aceitação e popularidade do site.</t>
-  </si>
-  <si>
-    <t>Usar o site, fornecer feedback, compartilhar experiências.</t>
-  </si>
-  <si>
-    <t>Manter os usuários satisfeitos, garantir que o site atenda às suas pesquisas.</t>
-  </si>
-  <si>
-    <t>Comunicar via e-mail, qualquer alteração ou novidade do produto e futuras ofertas</t>
-  </si>
-  <si>
-    <t>Fundamental para o sucesso do site.</t>
-  </si>
-  <si>
-    <t>Relatórios detalhados com métricas específicas e análise de tendências e escolhas.</t>
-  </si>
-  <si>
-    <t>Weekly durante a sprint e as demais reuniões do scrum.</t>
-  </si>
-  <si>
-    <t>O usuário visualizar e escolher o que melhor atende sua necessidade no momento de realizar uma corrida poraplicativo.</t>
-  </si>
-  <si>
-    <t>E-mails de ativação, engajamento, recorrência, news e comunicados gerais.</t>
-  </si>
-  <si>
-    <t>Desenvolver um site bem-sucedido que atenda às necessidades dos clientes.</t>
-  </si>
-  <si>
-    <t>Lançamento bem-sucedido, aumento de usuários ativos, satisfação dos clientes.</t>
-  </si>
-  <si>
-    <t>Sucesso do produto, inovação no mecado de comparadores de preços.</t>
-  </si>
-  <si>
-    <t>Relatórios de desempenho do site, métricas-chave, feedback dos usuários, status do desenvolvimento.</t>
-  </si>
-  <si>
-    <t>Reuniões semanais e mensais de revisão de desempenho.</t>
+Prototipação de produtos.</t>
+  </si>
+  <si>
+    <t>Reuniões virtuais e dados no GitHub e Figa</t>
+  </si>
+  <si>
+    <t>Mantêm os clientes satisfeitos e para os clientes e sentirem que seus problemas foram ouvidos e solucionados da melhor forma possível.</t>
+  </si>
+  <si>
+    <t>Responder a perguntas, resolver problemas, coletar feedback do cliente, relatório de problemas mensais.</t>
   </si>
 </sst>
 </file>
@@ -6992,11 +6992,11 @@
   <dimension ref="A1:M39"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="14" topLeftCell="B24" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="14" topLeftCell="C22" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
       <selection pane="topRight" activeCell="B4" sqref="B4"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="C24" sqref="C24"/>
+      <selection pane="bottomRight" activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7018,7 +7018,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="119" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
       <c r="B1" s="119"/>
       <c r="C1" s="119"/>
@@ -7030,16 +7030,16 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="103" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
       <c r="B2" s="100" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
       <c r="C2" s="103" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
       <c r="D2" s="100" t="s">
-        <v>239</v>
+        <v>228</v>
       </c>
       <c r="E2" s="100"/>
       <c r="F2" s="100"/>
@@ -7048,16 +7048,16 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="103" t="s">
-        <v>230</v>
+        <v>220</v>
       </c>
       <c r="B3" s="100" t="s">
-        <v>236</v>
+        <v>225</v>
       </c>
       <c r="C3" s="103" t="s">
-        <v>233</v>
+        <v>223</v>
       </c>
       <c r="D3" s="100" t="s">
-        <v>238</v>
+        <v>227</v>
       </c>
       <c r="E3" s="100"/>
       <c r="F3" s="100"/>
@@ -7166,16 +7166,16 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" s="103" t="s">
-        <v>231</v>
+        <v>221</v>
       </c>
       <c r="B14" s="100" t="s">
-        <v>237</v>
+        <v>226</v>
       </c>
       <c r="C14" s="103" t="s">
-        <v>234</v>
+        <v>278</v>
       </c>
       <c r="D14" s="104">
-        <v>45361</v>
+        <v>45726</v>
       </c>
       <c r="E14" s="100"/>
       <c r="F14" s="100"/>
@@ -7204,7 +7204,7 @@
       <c r="G16" s="114"/>
       <c r="H16" s="115"/>
       <c r="I16" s="116" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="J16" s="117"/>
       <c r="K16" s="117"/>
@@ -7216,10 +7216,10 @@
         <v>160</v>
       </c>
       <c r="B17" s="105" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="C17" s="105" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
       <c r="D17" s="106" t="s">
         <v>161</v>
@@ -7234,22 +7234,22 @@
         <v>164</v>
       </c>
       <c r="H17" s="106" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
       <c r="I17" s="106" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="J17" s="106" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
       <c r="K17" s="106" t="s">
-        <v>207</v>
+        <v>197</v>
       </c>
       <c r="L17" s="106" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="M17" s="106" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
     </row>
     <row r="18" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.2">
@@ -7257,60 +7257,60 @@
         <v>165</v>
       </c>
       <c r="B18" s="101" t="s">
-        <v>273</v>
+        <v>255</v>
       </c>
       <c r="C18" s="101" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="D18" s="101" t="s">
-        <v>274</v>
+        <v>280</v>
       </c>
       <c r="E18" s="101" t="s">
-        <v>275</v>
+        <v>256</v>
       </c>
       <c r="F18" s="101" t="s">
-        <v>276</v>
+        <v>257</v>
       </c>
       <c r="G18" s="101" t="s">
-        <v>277</v>
+        <v>258</v>
       </c>
       <c r="H18" s="101" t="s">
-        <v>278</v>
+        <v>259</v>
       </c>
       <c r="I18" s="101" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="J18" s="101" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
       <c r="K18" s="101" t="s">
-        <v>279</v>
+        <v>260</v>
       </c>
       <c r="L18" s="101" t="s">
-        <v>245</v>
+        <v>232</v>
       </c>
       <c r="M18" s="101" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="19" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="102" t="s">
-        <v>250</v>
+        <v>237</v>
       </c>
       <c r="B19" s="101" t="s">
-        <v>285</v>
+        <v>264</v>
       </c>
       <c r="C19" s="101" t="s">
-        <v>286</v>
+        <v>265</v>
       </c>
       <c r="D19" s="101" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="E19" s="101" t="s">
         <v>166</v>
       </c>
       <c r="F19" s="101" t="s">
-        <v>280</v>
+        <v>261</v>
       </c>
       <c r="G19" s="101" t="s">
         <v>167</v>
@@ -7319,19 +7319,19 @@
         <v>168</v>
       </c>
       <c r="I19" s="101" t="s">
-        <v>288</v>
+        <v>266</v>
       </c>
       <c r="J19" s="101" t="s">
-        <v>281</v>
+        <v>262</v>
       </c>
       <c r="K19" s="101" t="s">
-        <v>289</v>
+        <v>267</v>
       </c>
       <c r="L19" s="101" t="s">
-        <v>282</v>
+        <v>263</v>
       </c>
       <c r="M19" s="101" t="s">
-        <v>242</v>
+        <v>229</v>
       </c>
     </row>
     <row r="20" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.2">
@@ -7357,33 +7357,33 @@
         <v>174</v>
       </c>
       <c r="H20" s="101" t="s">
-        <v>248</v>
+        <v>235</v>
       </c>
       <c r="I20" s="101" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
       <c r="J20" s="101" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="K20" s="101" t="s">
-        <v>249</v>
+        <v>236</v>
       </c>
       <c r="L20" s="101" t="s">
-        <v>246</v>
+        <v>233</v>
       </c>
       <c r="M20" s="101" t="s">
-        <v>247</v>
+        <v>234</v>
       </c>
     </row>
     <row r="21" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="102" t="s">
-        <v>257</v>
+        <v>244</v>
       </c>
       <c r="B21" s="101" t="s">
-        <v>251</v>
+        <v>238</v>
       </c>
       <c r="C21" s="101" t="s">
-        <v>252</v>
+        <v>239</v>
       </c>
       <c r="D21" s="101" t="s">
         <v>176</v>
@@ -7395,25 +7395,25 @@
         <v>178</v>
       </c>
       <c r="G21" s="101" t="s">
-        <v>253</v>
+        <v>240</v>
       </c>
       <c r="H21" s="101" t="s">
         <v>179</v>
       </c>
       <c r="I21" s="101" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="J21" s="101" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="K21" s="101" t="s">
-        <v>254</v>
+        <v>241</v>
       </c>
       <c r="L21" s="101" t="s">
-        <v>255</v>
+        <v>242</v>
       </c>
       <c r="M21" s="101" t="s">
-        <v>243</v>
+        <v>230</v>
       </c>
     </row>
     <row r="22" spans="1:13" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -7421,40 +7421,40 @@
         <v>180</v>
       </c>
       <c r="B22" s="101" t="s">
-        <v>258</v>
+        <v>283</v>
       </c>
       <c r="C22" s="101" t="s">
-        <v>259</v>
+        <v>245</v>
       </c>
       <c r="D22" s="101" t="s">
         <v>181</v>
       </c>
       <c r="E22" s="101" t="s">
-        <v>260</v>
+        <v>284</v>
       </c>
       <c r="F22" s="101" t="s">
-        <v>261</v>
+        <v>246</v>
       </c>
       <c r="G22" s="101" t="s">
         <v>182</v>
       </c>
       <c r="H22" s="101" t="s">
-        <v>262</v>
+        <v>285</v>
       </c>
       <c r="I22" s="101" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="J22" s="101" t="s">
-        <v>263</v>
+        <v>247</v>
       </c>
       <c r="K22" s="101" t="s">
-        <v>264</v>
+        <v>248</v>
       </c>
       <c r="L22" s="101" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="M22" s="101" t="s">
-        <v>271</v>
+        <v>254</v>
       </c>
     </row>
     <row r="23" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.2">
@@ -7462,10 +7462,10 @@
         <v>183</v>
       </c>
       <c r="B23" s="101" t="s">
-        <v>266</v>
+        <v>286</v>
       </c>
       <c r="C23" s="101" t="s">
-        <v>265</v>
+        <v>249</v>
       </c>
       <c r="D23" s="101" t="s">
         <v>184</v>
@@ -7477,107 +7477,107 @@
         <v>186</v>
       </c>
       <c r="G23" s="101" t="s">
-        <v>267</v>
+        <v>250</v>
       </c>
       <c r="H23" s="101" t="s">
-        <v>268</v>
+        <v>251</v>
       </c>
       <c r="I23" s="101" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
       <c r="J23" s="101" t="s">
-        <v>219</v>
+        <v>209</v>
       </c>
       <c r="K23" s="101" t="s">
-        <v>269</v>
+        <v>252</v>
       </c>
       <c r="L23" s="101" t="s">
-        <v>270</v>
+        <v>253</v>
       </c>
       <c r="M23" s="101" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A24" s="102" t="s">
-        <v>256</v>
+        <v>243</v>
       </c>
       <c r="B24" s="101" t="s">
         <v>187</v>
       </c>
       <c r="C24" s="101" t="s">
-        <v>188</v>
+        <v>268</v>
       </c>
       <c r="D24" s="101" t="s">
-        <v>189</v>
+        <v>272</v>
       </c>
       <c r="E24" s="101" t="s">
-        <v>190</v>
+        <v>269</v>
       </c>
       <c r="F24" s="101" t="s">
-        <v>191</v>
+        <v>288</v>
       </c>
       <c r="G24" s="101" t="s">
-        <v>192</v>
+        <v>289</v>
       </c>
       <c r="H24" s="101" t="s">
-        <v>193</v>
+        <v>273</v>
       </c>
       <c r="I24" s="101" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
       <c r="J24" s="101" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
       <c r="K24" s="101" t="s">
-        <v>241</v>
+        <v>274</v>
       </c>
       <c r="L24" s="101" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
       <c r="M24" s="101" t="s">
-        <v>244</v>
+        <v>231</v>
       </c>
     </row>
     <row r="25" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="102" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="B25" s="101" t="s">
-        <v>195</v>
+        <v>270</v>
       </c>
       <c r="C25" s="101" t="s">
-        <v>196</v>
+        <v>275</v>
       </c>
       <c r="D25" s="101" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="E25" s="101" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="F25" s="101" t="s">
-        <v>199</v>
+        <v>271</v>
       </c>
       <c r="G25" s="101" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="H25" s="101" t="s">
-        <v>201</v>
+        <v>276</v>
       </c>
       <c r="I25" s="101" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
       <c r="J25" s="101" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
       <c r="K25" s="101" t="s">
-        <v>240</v>
+        <v>277</v>
       </c>
       <c r="L25" s="101" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="M25" s="101" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">

</xml_diff>